<commit_message>
update:se modifica headless para trabajar en segundo plano(rex)
</commit_message>
<xml_diff>
--- a/NOVEDADES_COMERCIALES.xlsx
+++ b/NOVEDADES_COMERCIALES.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YULYCO~1\AppData\Roaming\MobaXterm\slash\mx86_64b\RemoteFiles\133238_2_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jeico\bot-novedades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD95465-B56F-49FF-8AFE-B01BBDED9B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73AFBEE-1D51-49F3-B53F-B4E87396EEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5AE651C2-1F96-4DC5-8236-A1DBC4D9C962}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Código TdC</t>
   </si>
@@ -71,12 +71,6 @@
     <t>MCS30 3X277/480V CL 0,5 5-10</t>
   </si>
   <si>
-    <t>ENEL</t>
-  </si>
-  <si>
-    <t>CERT3-I(5/100A) 3X120/208V Cl. 1</t>
-  </si>
-  <si>
     <t>HEXING</t>
   </si>
   <si>
@@ -87,18 +81,6 @@
   </si>
   <si>
     <t>3X(58/100....277/480V), 10-160A, CL1, 6E-2D</t>
-  </si>
-  <si>
-    <t>NINGBO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N23U03 (2X120/208) 5-100A, CL 1, 5E-2D </t>
-  </si>
-  <si>
-    <t>HXE34K CONX. DIRECTA 5(120)A, 5.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N34U03 (3X120/208V), 5-100A, CL1, 6E2D </t>
   </si>
   <si>
     <t>IT0009 - Instalación</t>
@@ -111,58 +93,6 @@
 SE REALIZAN PRUEBAS A MACRO INSTALADO LAS CUALES SON CONFORMES RELACION DE CTS 1000:5 OK  SE INSTALA  @JUEGODECTSFX200×3 @CONECTORES @BP @CABLE12×12 @PERNOMARGARITA @CABLEFLEX#12 @CONJUNTODECIERR AL FINALIZAR TODO QUEDA EN CORRECTO FUNCIONAMIENTO SE TOMAN FOTOS</t>
   </si>
   <si>
-    <t>TROUBLESHOOTING CLIENTE INSPECCION CUENTA SMART, MEDIDOR PERDIO COMUNICACION CON EL CONCENTRADOR SE ENCUENTRA  CELDA NORMALIZADA TRIFASICA COMUNICACIÓN EN FALLA ACOMETIDA 3×8 AWG POTENCIA INSTATANIA 0.36 KW SE REALIZA PRUEBA DE FUNCIONAMIENTO CON CARGA RESITIVA DANDO  AL -100% DE ERROR  MEDIDOR BLOQUEADO  PRESTA SERVICIO A VIVIENDA  REALIZA RESET AL MEDIDOR  NO RESPODEN SE REALIZA CAMBIO DE MEDIDOR SE RESTABLECE COMUNICACIÓN CON CGM CGM CÓDIGO: SM 51681 MEDIDOR RETIRADO ES ENVIADO EN CADENA DE CUSTODIA PARA SU DICTAME SE ENTRAGA CARTA DE CAMBIO  INSTALACIÓN QUEDA FUNCIONANDO COMO SE ENCONTRO PRUEBAS FINALES DANDO DENTRO DEL RANGO SE TOMA REGISTRO FOTOGRÁFICO</t>
-  </si>
-  <si>
-    <t>INSPECCION LV. SE ENCUENTRA CLIENTE CON EL SERVICIO SUSPENDIDO DESDE CC. SE REALIZA RECONEXION DEL SERVICIO DESDE MEDIDOR CON ORDEN ENEL YA QUE CLIENTE PERMITE REALIZAR INSPECCION INTEGRAL Y CAMBIO DE MEDIDOR. POTENCIA INSTANTANEA 0.16 KW. ACOMETIDA NO 8 DESDE BARRAJE. MEDIDOR EXTERNO ARMARIO 12 CUENTAS. USO VIVIENDA. AFORO REALIZADO. SIN SELLO EN CC 1D1. PRUEBAS A MEDIDOR DAN BAJO PORCENTAJE DE REGISTRO. SE RETIRA MEDIDOR EN KIT DE CUSTODIA PARA SU DICTAMEN EN LABORATORIO. COMUNICARSEAL 5140000 SI DESEA ESTAR PRESENTE EN EL DICTAMEN. SE ENTREGA CARTA. PRUEBAS A MEDIDOR INTALADO DENTRO DEL RANGO. SE ANEXAN FOTOS.</t>
-  </si>
-  <si>
-    <t>INSPECCIÓN PARA VALIDAR ESTADO Y FUNCIONAMIENTO DE LA MEDIDA, SE LLEGA A PREDIO, SE ENCUENTRA MEDIDOR EN CELDA MINI MANTIS A LA ALTURA DE LA RED DE BT, ACOM 3×8+10 AWG P.INST 15 KW, SE REALIZAN PRUEBAS DE FUNCIONAMIENTO AL MEDIDOR CON CARGA DEL PREDIO, PRUEBAS POR DEBAJO DEL RANGO, BAJO PORCENTAJE REGISTRADO POR EL MEDIDOR, SE EVIDENCIA MEDIDOR QUEMADO A LA ENTRADA DE LA FASE R, SE EXPLICA PROCEDIMIENTO A PERSONA QUE ATIENDE, SE CAMBIA MEDIDOR, SE CAMBIA E INSTALA REPETIDOR, SE REALIZAN PRUEBAS DE FUNCIONAMIENTO, PRUEBAS OK DENTRO DEL RANGO, SE HACE USO DE STARBEAT, @TELEMEDIDA OK, SE DEJA EL MISMO SISTEMA DE COMUNICACIÓN ENCONTRADO, SE REALIZA @AFORO, MEDIDA PRESTA SERVICIO A AUTOLAVADO EL TABOR, REPETIDOR QUEDA DANDO LECTURA OK, AL FINALIZAR QUEDA TODO OK, SEÑOR USUARIO TIENE DOS DÍAS HÁBILES PARA AGENDAR Y ESTAR PRESENTE EN DICTAMEN DE LABORATORIO, PARA AGENDAR COMUNIQUESE A LA LÍNEA ENEL 6015140000. SE ENTREGA CARTA CAMBIO DE MEDIDOR, SE ANEXA REGISTRO FOTOGRAFICO.</t>
-  </si>
-  <si>
-    <t>INSPECCION SOLICITADA POR EL CLIENTE PARA VERIFICAR ESTADO Y FUNCIONAMIENTO DEL MEDIDOR OBS TRR CELDA EXTERNA 1 CUENTA ACOMETIDA 2X8 AWG AÉREA POT INS 0.21KW PRESTA SERVICIO A VIVIENDA PERSONA QUE ATIENDE MANIFIESTA QUE LE A ESTADO SUBIENDO EL CONSUMO. PRUEBAS AL MEDIDOR PRESENTANDO FALLAS MEDIDOR REGISTRA ALTO PORCENTAJE MEDIDOR REGISTRA SIN CARGA. SE EXPLICA PROCEDIMIENTO. SE RETIRA MEDIDOR EN TULA TRASPARENTE AL LABORATORIO SEÑOR USUARIO SI DESEA ESTAR PRESENTE EN EVALUACIÓN DE ELEMENTO COMUNICARSE A LA LÍNEA 5140000 EN LOS SIGUIENTES 2 DÍAS HÁBILES DESPUÉS DEL CAMBIO. MEDIDOR INSTALADO A PRUEBAS CONFORMES. TODOS LOS EQUIPOS QUEDAN A SATISFACCIÓN DEL USUARIO. VISOR OPACO SE REALIZA CAMBIO PARA NORMALIZAR LA TOMA DE LECTURAS @MMTCAJA SE EXPLICA A USUARIO QUE LOS COBROS SERÁN POR MEDIO DE LA FACTURA. SE ENTREGA CARTA. SE ANEXAN FOTOS</t>
-  </si>
-  <si>
-    <t>INSPECCION PARA CAMBIO DE MEDIDOR POR HALLAZGOS REPORTADOS EN ORDEN ANTERIOR OBS TRR ARMARIO INTERNO 12 CUENTAS ACOMETIDA 2X8 POT INS 0.11 KW PRESTA SERVICIO A VIVIENDA. MEDIDOR NO EMITE PULSOS REGISTRA BAJO PORCENTAJE. SE EXPLICA PROCEDIMIENTO. SE RETIRA MEDIDOR EN TULA TRASPARENTE AL LABORATORIO SEÑOR USUARIO SI DESEA ESTAR PRESENTE EN EVALUACIÓN DE ELEMENTO COMUNICARSE A LA LÍNEA 5140000 EN LOS SIGUIENTES 2 DÍAS HÁBILES DESPUÉS DEL CAMBIO. MEDIDOR INSTALADO A PRUEBAS CONFORMES. TODOS LOS EQUIPOS QUEDAN A SATISFACCIÓN DEL USUARIO. SE ENTREGA CARTA, CLIENTE SE AUSENTA AL MOMENTO DE DILIGENCIAMIENTO DE ACTA. SE ANEXAN FOTOS</t>
-  </si>
-  <si>
-    <t>LEET, INSTALACIÓN DE EQUIPO MOL, POT INST 2 KW, MED ELECTROM CON 5 ENT 1 DEC CON LECT ACT; 12366.5 KWH FX 1 ACOMETIDA 3X4 AWG CU ABIERTA DESDE BARRAGE, SE REALIZAN PRUEBAS MANUALES MÁS CARGA DEL PREDIO Y SIMULADOR DE CARGA DENTRO DEL RANGO, MEDIDOR PRESTA SERVICIO A ÁREAS COMUNES DE EDIFICIO  PORTELLO, SIN SELLOS 2 DE 2 EN ARMARIO, SE RETIRA MEDIDOR PARA SER ENVIADO A LABORATORIO, CLIENTE CUENTA CON DOS DÍAS HÁBILES PARA COMUNICARSE PARA SABER HORA Y FECHA DE DICTAMEN DEL MISMO, SE DEJA CARTA DE CAMBIO DE MEDIDOR, SE LE INFORMA AL CLIENTE QIE EL.CAMBIO DE MEDIDOR 39635067 CUALQUIER COBRO SE GENERARÁ EN LA FACTURA, SE AFORA, SE INSTALA MED 25010256 MODEM.SD&amp;CD01128, UNA CAJA PLC PARA EQUIPO DE COMUNICACIÓN SE CREA CUENTA EN STAR BEAT Y TELEMEDIDA QUEDA FUNC.OK, TIEMPO DE LA INSPECCIÓN DEBIDO A ESPERA DE AUTORIZACIÓN PARA CAMBIO DE MEDIDOR, MAY INF AL 5140000 ENEL COLOMBIA.</t>
-  </si>
-  <si>
-    <t>INSPECCIÓN INTEGRAL PARA VERIFICAR ESTADO Y FUNCIONAMIENTO DEL MEDIDOR MONOFASICO, PRUEBAS DE FUNCIONAMIENTO CON CARHA RESISTIVA, MEDIDOR NO REGISTRA, LED NO EMITE PULSOS, PORCE DE ERROR _-100_%, MEDIDOR QUEMADO, SERVICIO DIRECTO POR AE, POTENCIA INSTANTÁNEA 0.14 KW, MEDIDOR PARA USO DE VIVIENDA, SE INFORMA A CLIENTE, SE PROCEDE A CAMBIARLO, SE INSTALA 2 METROS DE CABLE PARA EMPALMAR ACOMETIDA Y DERIVACION DE MEDIDOR A PIN @MMTACO SE RETIRA EMPALMES,  MEDIDOR INSTALADO FUNCIONA DENTRO DE LO NORMAL, CELDA EXTERNA NORMALIZADO PARA 3 CUENTAS, NO SE SELLA, ACOMETIDA 2X8 LINEA ABIERTA DESDE POSTE, TODO QUEDA FUNCIONANDO EN CONDICIONES NORMALES, SE REALIZA AFORO, SEÑOR USUARIO COMUNICARSE A LA LINEA 5140000 PARA PRUEBAS DE LABORATORIO SI LO REQUIERE, SE ENTREGA CARTA DE CAMBIO  DE MEDIDOR SE ANEXAN FOTOS.</t>
-  </si>
-  <si>
-    <t>ATJG/A.A.INSPECCION A SOLICITUD DEL CLIENTE SE ENCUENTRA MEDIDOR INTERNO UBICADO EN ARMARIO PRESTA SERVICIO A VIVIENDA SE ENCUENTRA MEDIDOR EN SERVICIO DIRECTO DEJADO POR ATENCIÓN DE EMERGENCIAS. MEDIDOR CON BORNERO DE FASES  QUEMADO NO SE REALIZAN PRUEBAS POR RIESGO ELÉCTRICO SE EXPLICAN PROCEDIMIENTOS CLIENTE ACEPTA COSTOS SE PROCEDE CON CAMBIO DE MEDIDOR. MED INSTALADO #11492 MARCA 75. NIGBO SE REALIZAN PRUEBAS A MEDIDOR INSTALADO  DANDO NORMALES. SE REALIZA MANTENIMIENTO ACOMETIDA @MMTACO SE REALIZA @AFORO . SE ENTREGA CARTA DE CAMBIO, SEÑOR USUARIO SI DESEA ESTAR PRESENTE EN DICTAMEN DE LABORATORIO COMUNICARSE CON  LÍNEA DE ATENCIÓN ENEL601(5140000) EN PRÓXIMOS 2 DÍAS HÁBILES. SE TOMAN FOTOS.</t>
-  </si>
-  <si>
-    <t>A.M, DTO DE INSPECCIONES TÉCNICAS, B.S, OBS TRR.., VISITA POR SOLICITUD DE CLIENTE, MEDIDOR MONOFASICO, ORDEN CLIENTE OBJETIVO, FUNCIONA VIVIENDA MAS LOCAL SALON DE BELLEZA, CELDA DE MEDIDOR EXTERNA 4 CUENTAS NORMALIZADA, SE CAMBIA @VISOR@ ACOMETIDA #8 LINEA ABIERTA DESDE BARRAJE, SIN SELLO EN CC 1/1, POT INSTT 0.14 KW, MEDIDOR REGISTRANDO ALTO PORCENTAJE, REGISTRA SIN CARGA, SE REALIZA CAMBIO DE MEDIDOR, SE INSTALA EL MEDIDOR # 28336364 MARCA 117 HEXING MONOFASICO CON LECTURA ACTIVA 1.075 Y REACTIVA 0.580, MEDIDOR CONFORME A PRUEBAS, REGISTRANDO DENTRO DEL RANGO NORMAL, SE REALIZA AFORO, APLICA CAMBIO DE MODALIDAD A COMERCIAL YA QUE EL AFORO COMERCIAL SUPERA LOS 3 KW SIN CONEXIONAD, FAVOR ACTUALIZAR EN SISTEMA, SE ENTREGA CARTA DE NOTIFICACIÓN DE CAMBIO, SR USUARIO SI DESEA ESTAR PRESENTE EN PRUEBAS DE LABORATORIO DE MEDIDOR RETIRADO COMUNICARSE AL # 5140000 Y COORDINAR CITA ANTES DE 2 DÍAS, CLIENTE ACEPTA COSTOS POR VISOR, TODO QUEDA FUNCIONANDO CON NORMALIDAD, SE TOMAN FOTOS.</t>
-  </si>
-  <si>
-    <t>INSPECCION INTEGRAL PARA VERIFICAR ESTADO Y FUNCIONAMIENTO DEL MEDIDOR OBS TRR ARMARIO EXTERNO 20 CUENTAS ACOMETIDA 2X8 DESDE BARRAJE POT INS 0.04KW PRESTA SERVICIO A APARTAMENTO. MEDIDOR ELECTRÓNICO CON DISPLAY APAGADO LECTURA ILEGIBLE. MEDIDOR NO REGISTRA. SE EXPLICA PROCEDIMIENTO. SE RETIRA MEDIDOR EN TULA TRASPARENTE AL LABORATORIO SEÑOR USUARIO SI DESEA ESTAR PRESENTE EN EVALUACIÓN DE ELEMENTO COMUNICARSE A LA LÍNEA 5140000 EN LOS SIGUIENTES 2 DÍAS HÁBILES DESPUÉS DEL CAMBIO. MEDIDOR INSTALADO A PRUEBAS CONFORMES. TODOS LOS EQUIPOS QUEDAN A SATISFACCIÓN DEL USUARIO. SE ENTREGA CARTA. SE ANEXAN FOTOS</t>
-  </si>
-  <si>
-    <t>INSPECCION INTEGRAL PARA VERIFICAR ESTADO Y FUNCIONAMIENTO DEL MEDIDOR OBS TRR ARMARIO INTERNO 7 CUENTAS ACOMETIDA 3X8+10 DESDE BARRAJE POT 0.01KW PRESTA SERVICIO A APARTAMENTO. MEDIDOR ELECTRÓNICO CON DISPLAY APAGADO LECTURAS ILEGIBLES. MEDIDOR NO REGISTRA. SE EXPLICA PROCEDIMIENTO. SE RETIRA MEDIDOR EN TULA TRASPARENTE AL LABORATORIO SEÑOR USUARIO SI DESEA ESTAR PRESENTE EN EVALUACIÓN DE ELEMENTO COMUNICARSE A LA LÍNEA 5140000 EN LOS SIGUIENTES 2 DÍAS HÁBILES DESPUÉS DEL CAMBIO. MEDIDOR INSTALADO A PRUEBAS CONFORMES. TODOS LOS EQUIPOS QUEDAN A SATISFACCIÓN DEL USUARIO. SE RESTABLECE TELEMEDIDA CON GCM CODIGO (SM51682). SE ENTREGA CARTA. SE ANEXAN FOTOS</t>
-  </si>
-  <si>
-    <t>INSPECCION INTEGRAL PARA VERIFICAR ESTADO Y FUNCIONAMIENTO DEL MEDIDOR OBS TRR CELDA EXTERNA 2 CUENTAS ACOMETIDA 2X8 POT INS 0.52KW PRESTA SERVICIO A VIVIENDA. MEDIDOR ELECTRÓNICO CON DISPLAY BLOQUEADO ARROJANDO LECTURA ACTIVA LECTURA REACTIVA ILEGIBLE. MEDIDOR NO REGISTRA. SE EXPLICA PROCEDIMIENTO. SE RETIRA MEDIDOR EN TULA TRASPARENTE AL LABORATORIO SEÑOR USUARIO SI DESEA ESTAR PRESENTE EN EVALUACIÓN DE ELEMENTO COMUNICARSE A LA LÍNEA 5140000 EN LOS SIGUIENTES 2 DÍAS HÁBILES DESPUÉS DEL CAMBIO. MEDIDOR INSTALADO A PRUEBAS CONFORMES. TODOS LOS EQUIPOS QUEDAN A SATISFACCIÓN DEL USUARIO. VISOR OPACO SE REALIZA CAMBIO PARA NORMALIZAR LA TOMA DE LECTURAS @MMTCAJA SE EXPLICA A USUARIO QUE LOS COBROS SERÁN POR MEDIO DE LA FACTURA. SE ENTREGA CARTA. SE ANEXAN FOTOS</t>
-  </si>
-  <si>
-    <t>INSPECCIÓN INTEGRAL PARA VERIFICAR ESTADO Y FUNCIONAMIENTO DEL MEDIDOR MONOFASICO, PRUEBAS DE FUNCIONAMIENTO CON CARHA RESISTIVA, MEDIDOR NO REGISTRA, LED NO EMITE PULSOS, PORCE DE ERROR _-100_%, POTENCIA INSTANTÁNEA 0.10 KW, MEDIDOR PARA USO DE GIMNASIO, SE INFORMA A CLIENTE, SE PROCEDE A CAMBIARLO, MEDIDOR INSTALADO FUNCIONA DENTRO DE LO NORMAL, CELDA EXTERNA NORMALIZADO PARA 4 CUENTAS, NO SE SELLA, ACOMETIDA 2X8 LINEA ABIERTA DESDE BARRAJE. TODO QUEDA FUNCIONANDO EN CONDICIONES NORMALES, SE REALIZA AFORO, SE DEBE ACTUALIZAR EN SISTEMA CAMBIO DE MODALIDAD  DE RESIDENCIAL A COMERCIAL AREA Y AFARO 100% COMERCIAL. SEÑOR USUARIO COMUNICARSE A LA LINEA 5140000 PARA PRUEBAS DE LABORATORIO SI LO REQUIERE, SE ENTREGA CARTA DE CAMBIO  DE MEDIDOR SE ANEXAN FOTOS.</t>
-  </si>
-  <si>
-    <t>INSPECCIÓN INTEGRAL PARA VERIFICAR ESTADO Y FUNCIONAMIENTO DEL MEDIDOR TRIFÁSICO, PRUEBAS DE FUNCIONAMIENTO CON CARHA RESISTIVA, MEDIDOR NO REGISTRA, DISCO FRENADO, PORCE DE ERROR _-100_%, POTENCIA INSTANTÁNEA 0.48 KW, MEDIDOR PARA USO DE VIVIENDA, SE INFORMA A CLIENTE, SE PROCEDE A CAMBIARLO, MEDIDOR INSTALADO FUNCIONA DENTRO DE LO NORMAL, CELDA INTERNO NORMALIZADO PARA 12 CUENTAS, NO SE SELLA, ACOMETIDA 4X8 LINEA ABIERTA DESDE BARRAJE, TODO QUEDA FUNCIONANDO EN CONDICIONES NORMALES, SE REALIZA AFORO, SEÑOR USUARIO COMUNICARSE A LA LINEA 5140000 PARA PRUEBAS DE LABORATORIO SI LO REQUIERE, SE ENTREGA CARTA DE CAMBIO  DE MEDIDOR SE ANEXAN FOTOS.</t>
-  </si>
-  <si>
-    <t>IT. UL-12 SA. INSPECCIÓN TECNICA PARA VERIFICAR ESTADO Y FUNCIONAMIENTO DEL MEDIDOR.. SE ENCUENTRA PREDIO CON MEDIDOR OBJETIVO QUEMADO EN BLOQUE  DE TERMINAÑES ENTRADA Y SALIDA DE NUETROS. NEUTRO DESCONECTADO  DEJADO POR ATENCION DE EMERGENCIA. CON POTENCIA INSTANTÁNEA 0.24KW. CELDA DE MEDIDA EXTERNA CON 2 CUENTAS.  PRESTA SERVICIO A VIVIENDA. SIN SELLO.EN CAJA DE CONEXIONES. MEDIDOR NO REGISTRA.... SE CAMBIA MEDIDOR Y SE ENVÍA AL LABORATORIO  EN TULA TRANSPARENTE
-  SEÑOR USUARIO CUENTA CON 2 DÍAS CALENDARIO PARA  COMUNICARSE   EN LA LÍNEA 601-5140000  DE ENEL-COLOMBIA. Y AGENDAR UNA.CITA SI DESEA ESTAR PRESENTE EN LA EVALÚACION.DEL MEDIDOR EN EL LABORATORIO  @MMTACO SE REALIZA MANTENIMIENTO DE ACOMETIDA ELIMINANDO EMPALMES. SEÑOR USUSARIO CUNTA CON 30 DÍAS CALENDARIO PARA REALIZAR ADECUACIONES OBLIGATORIAS SEGUN NOR.ATIVIDAD VIGENTE DE NO HACERLO SOPENA A LA SUSPENSIÓN  DEL SERVICIO  SEGUN CCU.  SE ENTREGA CARTA DE CAMBIO.  SE TOMA REGISTRO FOTOGRAFICO</t>
-  </si>
-  <si>
-    <t>A.M, DTO DE INSPECCIONES TÉCNICAS, B.S, OBS TRR.., VISITA EJECUTADA POR SOLICITUD DE CLIENTE, INSPECCIÓN INTEGRAL, MEDIDOR MONOFASICO, ORDEN CLIENTE OBJETIVO, FUNCIONA VIVIENDA, CELDA DE MEDIDOR EXTERNA 2 CUENTAS NORMALIZADA, SE REALZIA CAMBIO DE @VISOR@, ACOMETIDA 2X8+10 AWG CONCENTRICA AÉREA, SIN SELLO EN CM 1/1, POT INSTT 0.18 KW, SE REALIZAN PRUEBAS, MEDIDOR REGISTRANDO ALTO PORCENTAJE, SE REALIZA CAMBIO DE MEDIDOR, SE INSTALA EL MEDIDOR # 28336363 MARCA 117 HEXING MONOFASICO CON LECTURA ACTIVA 1.080 Y REACTIVA 0.580, MEDIDOR CONFORME A PRUEBAS, REGISTRANDO DENTRO DEL RANGO NORMAL, NO SE REALIZA AFORO NO HAY ACCESO, SE ENTREGA CARTA DE NOTIFICACIÓN DE CAMBIO, SR USUARIO SI DESEA ESTAR PRESENTE EN PRUEBAS DE LABORATORIO DE MEDIDOR RETIRADO COMUNICARSE AL # 5140000 Y COORDINAR CITA ANTES DE 2 DÍAS, CLIENTE ACEPTA COSTOS POR CAMBIO DE VISOR, TODO QUEDA FUNCIONANDO CON NORMALIDAD, SE TOMAN FOTOS.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INSPECCIÓN POR CUADRILLA LIVIANA FONOSERVICIO SE VALIDA ESTADO Y FUNCIONAMIENTO  DE MEDIDOR ACTIVIDAD ESTADO DE CONEXIÓN  SE GARANTIZA TOMA DE LECTURA CLIENTE INDICA FALLA DE MEDIDOR CELDA NORMALIZADA BIFAMILIAR DOS CUENTAS PRESTA SERVICIO RESIDENCIAL  BQ6 CASA 2 SE REALIZAN PRUEBAS CON CARGA RESISTIVA EQUIPO PATRÓN POTENCIA INSTAN 0.12 KW MEDIDOR NO EMITE IMPULSOS NO REGISTRA SE REALIZA CAMBIO DE COMPONENTE EN PRESENCIA DEL.CLIENTE REGISTRANDO E INTEGRANDO  SEÑOR USUARIO COMUNICARSE CON LÍNEA ATENCIÓN 5140000 AGENDAR CITA Y ESTAR PRESENTE  EN PRUEBAS DE DICTAMEN DE LABOARTORIO SE LE EXPLICA PROCEDIMIENTO  PARA MAYOR INFORMACIÓN WWW.ENEL.COM.CO  SE REALIZA @MMTACO CAMBIO DE VISOR DE CELDA GARANTIZANDO TOMA DE LECTURA @MMTACO CAMBIO DE TERMOMAGNETICO  MONOFASICO CLIENTE ACEPTA COSTOS Y CONDICIONES  SE ENTREGA CARTA CAMBIO DE MEDIDOR SE TOMA SOPORTE FOTOGRÁFICO </t>
-  </si>
-  <si>
     <t>observacion</t>
   </si>
   <si>
@@ -176,13 +106,31 @@
   </si>
   <si>
     <t>modelo medidor extraido</t>
+  </si>
+  <si>
+    <t>IT.RG/CR.MED BIC 2@ALTURA RED BT EN CELDA MANTIS NO BRINDA SEGURIDAD CELDA QUEMADA.ACOMETIDA 3X2 AWG,FUNCIONA EMPRESA DE PLASTICO,SE ENCONTRÓ MED QUEMADO DESCONECTADO CON DISPLAY APAGADO SE RELACIONA LECT ACT Y REACT EN CERO(0),NO SE RELACION SELLOS DE TAPA PRINCIPAL NI SELLOS DE CC POR MEDIDOR E INSTALACION QUEMADA,RP APAGADO,CABLE PAR TELEF AVERIADO, CAJA RP DETERIORADA SIN TAPA.PREDIO EN SERVICIO DIRECTO DEJADO POR ATENCIÓN DE EMERGENCIA RADICADO#202563804642 CON POT.INST.38.85KW PRUEBAS AL-100%,SE REALIZA AFORO,SE VALIDA TELEM APP AUTODIAG 2 TELEM EN FALLA,SE @RETIRAN @CELDAS ENCONTRADAS DE @RP Y @MED,SE NORMALIZA SERVICIO INSTALANDO 1@CELDA MANTIS Y 1@CAJA MONO,SE INSTALA MED PRUEBAS DANDO OK,SE @CAMBIA RTU Y SIMCARD SE @INSTALA 1@RTU:053055,@1SIMCARD #57101702405420313,@5MTS PAR TELEF,1@RP, @1TUBO 1/2", 6@MTS CINTA BANDI Y 4@HEBILLAS @4CONECTOR PERFO @5MTS CABLE 3X2,SE CORRIGE @TELEM TELEM QUEDA OK.SI DESEA ESTAR PRESENTE EN LABORATORIO LLAMAR 5140000.SE DEJA CARTA</t>
+  </si>
+  <si>
+    <t>INHEMETER</t>
+  </si>
+  <si>
+    <t>3F-4H 5/10A 0.5s</t>
+  </si>
+  <si>
+    <t>FALLA DE COMUNICACIÓN// INSPECCIÓN PARA CORREGIR FALLA DE TELEMEDIDA, SE ENCUENTRA MEDIDOR EN CELDA CLIENTE. FX 40 CTS 200/5, ACOM 3×4/0 AWG, P.INST 7 KW. MEDIDA PRESTA SERVICIO A BDG 2 ÉTICOS SERRANO GOMEZ, NO SE AFORA, SE HACEN PRUEBAS DE FUNCIONAMIENTO CON CARGAS DEL PREDIO DANDO DENTRO DEL RANGO, SE CAMBIA MODEM Y SIM, MEDIDOR NO COMUNICA, MED ENCONTRADO CON PUERTO DE COMUNICACIÓN BLOQUEADO, SE EXPLICA PROCEDIMIENTO A PERSONA QUE ATIENDE, SE CAMBIA MEDIDOR, SE CAMBIA E INSTALA SISTEMA DE TELEMEDIDA, USO DE STARBET V2, SE CREA CUENTA, @TELEMEDIDA OK. @MMTACO, SE INST. @MODEM RU.SD8CD01013, SIM.8957101702405420322. @MMCAJA, SE VERIFICA BANDEJA PARTE POSTERIOR PARA CONFIRMAR CONEXIONADO. AL FINALIZAR QUEDA TODO OK, SEÑOR USUARIO TIENE DOS DIAS HÁBILES PARA COMUNICARSE Y ESTAR PRESENTE EN DICTAMEN DE LABORATORIO, PARA AGEN COMUNIQUESE A LA LINΕΑ 6015140000, SE ENTREGA CARTA DE CAMBIO DE MEDIDOR, SE ANEXA REGISTRO FOTOGRÁFICO</t>
+  </si>
+  <si>
+    <t>INSPECCION INTEGRAL PARA VERIFICAR ESTADO Y FUNCIONAMIENTO DEL MEDIDOR OBS TRR ARMARIO INTERNO 5 CUENTAS ACOMETIDA 2X8 DESDE BARRAJE POT INS 0.06KW PRESTA SERVICIO A APARTAMENTO. MEDIDOR ELECTRÓNICO CON DISPLAY APAGADO LECTURA ILEGIBLE. MEDIDOR NO REGISTRA. SE EXPLICA PROCEDIMIENTO. SE RETIRA MEDIDOR EN TULA TRASPARENTE AL LABORATORIO SEÑOR USUARIO SI DESEA ESTAR PRESENTE EN EVALUACIÓN DE ELEMENTO COMUNICARSE A LA LÍNEA 5140000 EN LOS SIGUIENTES 2 DÍAS HÁBILES DESPUÉS DEL CAMBIO. MEDIDOR INSTALADO A PRUEBAS CONFORMES. TODOS LOS EQUIPOS QUEDAN A SATISFACCIÓN DEL USUARIO. SE ENTREGA CARTA. SE ANEXAN FOTOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INSPECCIÓN POR CUADRILLA LIVIANA FONO SERVICIO  SE VALIDA ESTADO Y FUNCIONAMIENTO  DE MEDIDOR ACTIVIDAD ESTADO DE CONEXIÓN  SE GARANTIZA LECTURA CLIENTE INDICA FALLA DE MEDIDOR CELDA INTERNA NORMALIZADA ACOMETIDA NÚMERO 8 AWG DESDE BARRAJE PRESTA SERVICIO RESIDENCIAL PRIMER PISO SE VALIDA MEDIDOR CON DISPLAY APAGADO BLOQUEADO LECTURA ILEGIBLE SE INGRESA LECTURA CERO POR EFECTOS DE IMPRESIÓN MEDIDOR NO REGISTRA NO EMITE IMPULSOS SE REALIZA CAMBIO DE COMPONENTE EN PRESENCIA DEL CLIENTE COMUNICARSE CON LÍNEA ATENCIÓN 5140000 AGENDAR CITA Y ESTAR PRESENTE EN PRUEBAS DE DICTAMEN DE LABORATORIO PARA MAYOR INFORMACIÓN WWW.ENEL.COM.CO  SE ENTREGA CARTA CAMBIO DE MEDIDOR SE TOMA SOPORTE FOTOGRÁFICO </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,14 +142,6 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -259,13 +199,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,12 +542,13 @@
   <dimension ref="A1:M62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="39" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.5703125" customWidth="1"/>
     <col min="10" max="10" width="22.28515625" bestFit="1" customWidth="1"/>
@@ -642,19 +582,19 @@
         <v>7</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -671,7 +611,7 @@
         <v>110394374</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F2" s="1">
         <v>10200705</v>
@@ -683,501 +623,267 @@
         <v>9</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>1029634265</v>
+        <v>1029856260</v>
       </c>
       <c r="B3" s="1">
-        <v>1508167345</v>
+        <v>1512630789</v>
       </c>
       <c r="C3" s="2">
-        <v>45880</v>
+        <v>45883</v>
       </c>
       <c r="D3" s="1">
-        <v>556127</v>
+        <v>308315</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F3" s="1">
-        <v>6020743</v>
+        <v>25020209</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>1029752967</v>
+        <v>1029783649</v>
       </c>
       <c r="B4" s="1">
-        <v>1510454949</v>
+        <v>1510844475</v>
       </c>
       <c r="C4" s="2">
-        <v>45880</v>
+        <v>45883</v>
       </c>
       <c r="D4" s="1">
-        <v>2334488</v>
+        <v>417379</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F4" s="1">
-        <v>28336371</v>
+        <v>37295538047</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>1029778023</v>
+        <v>1029820136</v>
       </c>
       <c r="B5" s="1">
-        <v>1510644065</v>
+        <v>1511682579</v>
       </c>
       <c r="C5" s="2">
-        <v>45880</v>
+        <v>45883</v>
       </c>
       <c r="D5" s="1">
-        <v>733277</v>
+        <v>2210888</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F5" s="1">
-        <v>25010267</v>
+        <v>28336903</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>1029782136</v>
+        <v>1029822590</v>
       </c>
       <c r="B6" s="1">
-        <v>1510691742</v>
+        <v>1511707327</v>
       </c>
       <c r="C6" s="2">
-        <v>45880</v>
+        <v>45883</v>
       </c>
       <c r="D6" s="1">
-        <v>2493619</v>
+        <v>561655</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F6" s="1">
-        <v>28336904</v>
+        <v>28336468</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>1029782152</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1510652575</v>
-      </c>
-      <c r="C7" s="2">
-        <v>45880</v>
-      </c>
-      <c r="D7" s="1">
-        <v>98167619</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="1">
-        <v>28336022</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>1029782154</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1510694017</v>
-      </c>
-      <c r="C8" s="2">
-        <v>45880</v>
-      </c>
-      <c r="D8" s="1">
-        <v>644473</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="1">
-        <v>25010265</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>1029782171</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1510693303</v>
-      </c>
-      <c r="C9" s="2">
-        <v>45880</v>
-      </c>
-      <c r="D9" s="1">
-        <v>2616329</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="1">
-        <v>28336016</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>1029782208</v>
-      </c>
-      <c r="B10" s="1">
-        <v>1510689428</v>
-      </c>
-      <c r="C10" s="2">
-        <v>45880</v>
-      </c>
-      <c r="D10" s="1">
-        <v>277230019</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="1">
-        <v>11492</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>1029783608</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1510801497</v>
-      </c>
-      <c r="C11" s="2">
-        <v>45880</v>
-      </c>
-      <c r="D11" s="1">
-        <v>2272064</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="1">
-        <v>28336364</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>1029791626</v>
-      </c>
-      <c r="B12" s="1">
-        <v>1510929297</v>
-      </c>
-      <c r="C12" s="2">
-        <v>45880</v>
-      </c>
-      <c r="D12" s="1">
-        <v>2105172</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="1">
-        <v>28336914</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>1029791817</v>
-      </c>
-      <c r="B13" s="1">
-        <v>1510929276</v>
-      </c>
-      <c r="C13" s="2">
-        <v>45880</v>
-      </c>
-      <c r="D13" s="1">
-        <v>744398</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="1">
-        <v>6022038</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>1029791875</v>
-      </c>
-      <c r="B14" s="1">
-        <v>1510929270</v>
-      </c>
-      <c r="C14" s="2">
-        <v>45880</v>
-      </c>
-      <c r="D14" s="1">
-        <v>2494591</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="1">
-        <v>28336906</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>1029793262</v>
-      </c>
-      <c r="B15" s="1">
-        <v>1510935527</v>
-      </c>
-      <c r="C15" s="2">
-        <v>45880</v>
-      </c>
-      <c r="D15" s="1">
-        <v>2373556</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="1">
-        <v>28336934</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>1029793263</v>
-      </c>
-      <c r="B16" s="1">
-        <v>1510936633</v>
-      </c>
-      <c r="C16" s="2">
-        <v>45880</v>
-      </c>
-      <c r="D16" s="1">
-        <v>1677822</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="1">
-        <v>23911442</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>1029793280</v>
-      </c>
-      <c r="B17" s="1">
-        <v>1510936724</v>
-      </c>
-      <c r="C17" s="2">
-        <v>45880</v>
-      </c>
-      <c r="D17" s="1">
-        <v>137591</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17" s="1">
-        <v>19135</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>1029793289</v>
-      </c>
-      <c r="B18" s="1">
-        <v>1510936888</v>
-      </c>
-      <c r="C18" s="2">
-        <v>45880</v>
-      </c>
-      <c r="D18" s="1">
-        <v>2401156</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F18" s="1">
-        <v>28336363</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>1029793297</v>
-      </c>
-      <c r="B19" s="1">
-        <v>1510965074</v>
-      </c>
-      <c r="C19" s="2">
-        <v>45880</v>
-      </c>
-      <c r="D19" s="1">
-        <v>2796516</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19" s="1">
-        <v>28336796</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>

</xml_diff>